<commit_message>
Moved most data manipulation to .py files in folder. Modeling is in Crew-rating_using_py_scripts notebook. Added icon ids to character data
</commit_message>
<xml_diff>
--- a/grades_comp.xlsx
+++ b/grades_comp.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="378">
   <si>
     <t>CharacterDesignName</t>
   </si>
@@ -1089,6 +1089,9 @@
   </si>
   <si>
     <t>Cupid Trooper</t>
+  </si>
+  <si>
+    <t>CharacterDesignId</t>
   </si>
   <si>
     <t>RaceType</t>
@@ -7548,18 +7551,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:U1"/>
+  <dimension ref="B1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:21">
+    <row r="1" spans="2:22">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>358</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>358</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>359</v>
@@ -7614,6 +7617,9 @@
       </c>
       <c r="U1" s="1" t="s">
         <v>376</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>